<commit_message>
Fix IRR error in analysis
</commit_message>
<xml_diff>
--- a/assets/worksheets/5yr-IRR-Analysis.xlsx
+++ b/assets/worksheets/5yr-IRR-Analysis.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nscho\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f86cf31dab8dac97/Documents/Work/Public Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D874F7FA-CF6E-4182-896C-6024C1272EDF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{CF6397A3-CAC9-40AE-8999-2BDA53F55A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="18930" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5YrAnalysis" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -158,7 +168,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.00&quot;x&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -187,11 +197,18 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +225,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -232,39 +255,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="32">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +617,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -599,81 +628,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4">
         <v>2800000</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f>C7</f>
         <v>1736000</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4">
         <v>56000</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4">
         <v>1736000</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4">
         <v>17360</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="8">
         <f>PMT(F6/12,F7*12,-F5)</f>
         <v>9319.2233754907338</v>
       </c>
@@ -687,16 +716,16 @@
         <f>C5+C6-C7+C8</f>
         <v>1137360</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="8">
         <f>F8*12</f>
         <v>111830.6805058888</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -708,39 +737,39 @@
       <c r="C12" s="13">
         <v>1</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="14">
         <f t="shared" ref="D12:G12" si="0">C12+1</f>
         <v>2</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15">
+      <c r="B13" s="3"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16">
         <v>0.03</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="16">
         <v>0.03</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="16">
         <v>0.03</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="16">
         <v>0.03</v>
       </c>
     </row>
@@ -748,23 +777,23 @@
       <c r="A14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5">
+      <c r="B14" s="3"/>
+      <c r="C14" s="4">
         <v>238800</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <f t="shared" ref="D14:G14" si="1">C14*(1+D13)</f>
         <v>245964</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <f t="shared" si="1"/>
         <v>253342.92</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
         <v>260943.20760000002</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>268771.50382800004</v>
       </c>
@@ -773,23 +802,23 @@
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5">
+      <c r="B15" s="3"/>
+      <c r="C15" s="4">
         <v>4540</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f t="shared" ref="D15:G15" si="2">C15*(1+D13)</f>
         <v>4676.2</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f t="shared" si="2"/>
         <v>4816.4859999999999</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <f t="shared" si="2"/>
         <v>4960.9805800000004</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f t="shared" si="2"/>
         <v>5109.8099974000006</v>
       </c>
@@ -798,52 +827,52 @@
       <c r="A16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3">
         <f t="shared" ref="C16:G16" si="3">C14+C15</f>
         <v>243340</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <f t="shared" si="3"/>
         <v>250640.2</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <f t="shared" si="3"/>
         <v>258159.40600000002</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <f t="shared" si="3"/>
         <v>265904.18818</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f t="shared" si="3"/>
         <v>273881.31382540002</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="18">
         <v>2.9399999999999999E-2</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="8">
         <f t="shared" ref="C17:G17" si="4">C16*$B$17</f>
         <v>7154.1959999999999</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="8">
         <f t="shared" si="4"/>
         <v>7368.8218800000004</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="8">
         <f t="shared" si="4"/>
         <v>7589.8865364000003</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="8">
         <f t="shared" si="4"/>
         <v>7817.583132492</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="8">
         <f t="shared" si="4"/>
         <v>8052.1106264667606</v>
       </c>
@@ -852,126 +881,126 @@
       <c r="A18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8">
         <f t="shared" ref="C18:G18" si="5">C16-C17</f>
         <v>236185.804</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="8">
         <f t="shared" si="5"/>
         <v>243271.37812000001</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="8">
         <f t="shared" si="5"/>
         <v>250569.51946360001</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="8">
         <f t="shared" si="5"/>
         <v>258086.605047508</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="8">
         <f t="shared" si="5"/>
         <v>265829.20319893328</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15">
+      <c r="B19" s="3"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16">
         <v>0.03</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="16">
         <v>0.03</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="16">
         <v>0.03</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="16">
         <v>0.03</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5">
+      <c r="B20" s="3"/>
+      <c r="C20" s="4">
         <v>87213</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <f t="shared" ref="D20:G20" si="6">C20*(1+D19)</f>
         <v>89829.39</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <f t="shared" si="6"/>
         <v>92524.271699999998</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f t="shared" si="6"/>
         <v>95299.999851</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" si="6"/>
         <v>98158.999846530001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20">
         <f t="shared" ref="C21:G21" si="7">C18-C20</f>
         <v>148972.804</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="20">
         <f t="shared" si="7"/>
         <v>153441.98811999999</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="20">
         <f t="shared" si="7"/>
         <v>158045.24776360003</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="20">
         <f t="shared" si="7"/>
         <v>162786.605196508</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="20">
         <f t="shared" si="7"/>
         <v>167670.20335240327</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8">
         <f t="shared" ref="C22:G22" si="8">$F$9</f>
         <v>111830.6805058888</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="8">
         <f t="shared" si="8"/>
         <v>111830.6805058888</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="8">
         <f t="shared" si="8"/>
         <v>111830.6805058888</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="8">
         <f t="shared" si="8"/>
         <v>111830.6805058888</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="8">
         <f t="shared" si="8"/>
         <v>111830.6805058888</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="10"/>
@@ -997,291 +1026,291 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21">
+      <c r="B25" s="22"/>
+      <c r="C25" s="22">
         <f>C21/C5</f>
         <v>5.3204572857142855E-2</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>5.3199999999999997E-2</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>5.3199999999999997E-2</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>5.3199999999999997E-2</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>5.3199999999999997E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="8">
         <f t="shared" ref="C26:G26" si="10">ROUND(C21/C25,-4)</f>
         <v>2800000</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="8">
         <f t="shared" si="10"/>
         <v>2880000</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="8">
         <f t="shared" si="10"/>
         <v>2970000</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="8">
         <f t="shared" si="10"/>
         <v>3060000</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="8">
         <f t="shared" si="10"/>
         <v>3150000</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8">
         <f t="shared" ref="C28:G28" si="11">$F$5+CUMPRINC($F$6/12,$F$7*12,$F$5,1,C12*12,0)</f>
         <v>1710387.6576009486</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="8">
         <f t="shared" si="11"/>
         <v>1683464.9391555649</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="8">
         <f t="shared" si="11"/>
         <v>1655164.8033383798</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="8">
         <f t="shared" si="11"/>
         <v>1625416.7788624768</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="8">
         <f t="shared" si="11"/>
         <v>1594146.7889961542</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22">
+      <c r="B29" s="23"/>
+      <c r="C29" s="23">
         <f t="shared" ref="C29:G29" si="12">C28/C26</f>
         <v>0.61085273485748159</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="23">
         <f t="shared" si="12"/>
         <v>0.58453643720679338</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="23">
         <f t="shared" si="12"/>
         <v>0.55729454657857902</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="23">
         <f t="shared" si="12"/>
         <v>0.53118195387662637</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="23">
         <f t="shared" si="12"/>
         <v>0.50607834571306487</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24">
+      <c r="B30" s="24"/>
+      <c r="C30" s="25">
         <f t="shared" ref="C30:G30" si="13">C21/C22</f>
         <v>1.3321282078056869</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="25">
         <f t="shared" si="13"/>
         <v>1.3720920540398573</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="25">
         <f t="shared" si="13"/>
         <v>1.4132548156610534</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="25">
         <f t="shared" si="13"/>
         <v>1.4556524601308847</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="25">
         <f t="shared" si="13"/>
         <v>1.4993220339348114</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="5">
+      <c r="B32" s="23"/>
+      <c r="C32" s="4">
         <v>0</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>0</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <v>0</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="4">
         <v>0</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="4">
+      <c r="B33" s="23"/>
+      <c r="C33" s="3">
         <f>C32+C9</f>
         <v>1137360</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <f t="shared" ref="D33:G33" si="14">D32+C33</f>
         <v>1137360</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <f t="shared" si="14"/>
         <v>1137360</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <f t="shared" si="14"/>
         <v>1137360</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <f t="shared" si="14"/>
         <v>1137360</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22">
+      <c r="B34" s="23"/>
+      <c r="C34" s="23">
         <f t="shared" ref="C34:G34" si="15">C23/C33</f>
         <v>3.2656435512160797E-2</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="23">
         <f t="shared" si="15"/>
         <v>3.6585872207666167E-2</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="23">
         <f t="shared" si="15"/>
         <v>4.0633192004036742E-2</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="23">
         <f t="shared" si="15"/>
         <v>4.4801931394298375E-2</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="23">
         <f t="shared" si="15"/>
         <v>4.9095732966267916E-2</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="8">
         <f t="shared" ref="C37:G37" si="16">C26</f>
         <v>2800000</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="8">
         <f t="shared" si="16"/>
         <v>2880000</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="8">
         <f t="shared" si="16"/>
         <v>2970000</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="8">
         <f t="shared" si="16"/>
         <v>3060000</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="8">
         <f t="shared" si="16"/>
         <v>3150000</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="18">
         <v>0.05</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="8">
         <f t="shared" ref="C38:G38" si="17">C37*$B$38</f>
         <v>140000</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="8">
         <f t="shared" si="17"/>
         <v>144000</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="8">
         <f t="shared" si="17"/>
         <v>148500</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="8">
         <f t="shared" si="17"/>
         <v>153000</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="8">
         <f t="shared" si="17"/>
         <v>157500</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="8">
         <f t="shared" ref="C39:G39" si="18">C28</f>
         <v>1710387.6576009486</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="8">
         <f t="shared" si="18"/>
         <v>1683464.9391555649</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="8">
         <f t="shared" si="18"/>
         <v>1655164.8033383798</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="8">
         <f t="shared" si="18"/>
         <v>1625416.7788624768</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="8">
         <f t="shared" si="18"/>
         <v>1594146.7889961542</v>
       </c>
@@ -1290,7 +1319,10 @@
       <c r="A40" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="9"/>
+      <c r="B40" s="28">
+        <f>-C9</f>
+        <v>-1137360</v>
+      </c>
       <c r="C40" s="10">
         <f t="shared" ref="C40:G40" si="19">C37-C38-C39</f>
         <v>949612.34239905141</v>
@@ -1313,78 +1345,83 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="30">
         <f>-C9</f>
         <v>-1137360</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="8">
         <f t="shared" ref="C41:G41" si="20">C23-C32</f>
         <v>37142.123494111205</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="8">
         <f t="shared" si="20"/>
         <v>41611.307614111196</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="8">
         <f t="shared" si="20"/>
         <v>46214.567257711227</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="8">
         <f t="shared" si="20"/>
         <v>50955.924690619198</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="8">
         <f t="shared" si="20"/>
         <v>55839.522846514476</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="8">
         <f t="shared" ref="C42:G42" si="21">C23-C32+C40</f>
         <v>986754.46589316265</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="8">
         <f t="shared" si="21"/>
         <v>1094146.3684585462</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="8">
         <f t="shared" si="21"/>
         <v>1212549.7639193314</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="8">
         <f t="shared" si="21"/>
         <v>1332539.1458281423</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="8">
         <f t="shared" si="21"/>
         <v>1454192.7338503604</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="29" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="27">
-        <v>-0.13241676699999999</v>
+        <f>IRR(($B$41:B41,C42))</f>
+        <v>-0.13241676699271776</v>
       </c>
       <c r="D43" s="27">
-        <v>-2.717181523E-3</v>
+        <f>IRR(($B$41:C41,D42))</f>
+        <v>-2.7171815228642648E-3</v>
       </c>
       <c r="E43" s="27">
-        <v>4.4633066120000002E-2</v>
+        <f>IRR(($B$41:D41,E42))</f>
+        <v>4.4633066123451304E-2</v>
       </c>
       <c r="F43" s="27">
-        <v>6.7027693609999994E-2</v>
+        <f>IRR(($B$41:E41,F42))</f>
+        <v>6.7027693615650641E-2</v>
       </c>
       <c r="G43" s="27">
-        <v>7.9299313989999995E-2</v>
+        <f>IRR(($B$41:F41,G42))</f>
+        <v>7.9299313994779297E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>